<commit_message>
Solved recurrening departed issue. Important update where the issue of departed time keeps on changing is fixed. Now departed time is updated only once when the status is changed to departed.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15:45:17</t>
+          <t>16:33:29</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>15:45:26</t>
+          <t>16:33:36</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Important ERROR solved. In previous versions, even if a specific face appeared in non-consecutive frames, the program will still make it present which is a major flaw. To be more specific, the issue with the previous implementations is that the consecutive_frames_dict is simply counting the number of frames where the employee's face is detected, without considering whether they are consecutive or not. To ensure that an employee's status is changed to "present" only if their face is detected in 'max_consecutive_frames' consecutive frames, we need to modify the code to keep track of consecutive frames where their face is detected and update the status accordingly.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>16:33:29</t>
+          <t>19:58:53</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>16:33:36</t>
+          <t>19:58:58</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Continuously save excel file within loop. Here, instead of only saving changes to excel after quitting the program, whenever a change in status happens, it will always save these changes immedietaly without leaving the main loop.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -526,22 +526,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023-07-23</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>20:59:59</t>
+          <t>01:13:47</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-07-23</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>21:00:04</t>
+          <t>01:14:11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Time difference feature. Added a new key in the dictionary to calcualte the difference between time of arrival and departure. This will show in excel.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>departure_time</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>time_difference</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -480,6 +485,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -496,6 +502,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -512,6 +519,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -526,22 +534,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023-07-24</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>01:13:47</t>
+          <t>16:44:47</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-07-24</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>01:14:11</t>
+          <t>16:44:56</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0:00:09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
No face detected feature. Added text that says no face detected if there are none in frame and some simple refactoring.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>16:44:47</t>
+          <t>17:38:31</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -549,12 +549,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>16:44:56</t>
+          <t>17:38:35</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0:00:09</t>
+          <t>0:00:04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Very imp rafactoring. Now the detection for arrival and departure works as expected.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -534,27 +534,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023-07-25</t>
+          <t>2023-07-26</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17:45:56</t>
+          <t>14:31:14</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-07-25</t>
+          <t>2023-07-26</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>17:46:00</t>
+          <t>14:31:22</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0:00:04</t>
+          <t>0:00:08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Reset to absent if no departure. This new feature will reset employee status back to absent if he/she forgot to depart when finishing work.
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -529,7 +529,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>departed</t>
+          <t>absent</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,24 +539,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14:31:14</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2023-07-26</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>14:31:22</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0:00:08</t>
-        </is>
-      </c>
+          <t>15:35:13</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>